<commit_message>
start the home menu
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6E9606-E6E5-430C-B81C-8AA94061E4AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3A9BFF-B0A8-4D16-92C7-E7E20A1E06C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>https://www.figma.com/file/bxToUy6ylJsOtMk0nXZpcq/Untitled?type=design&amp;node-id=0%3A1&amp;mode=design&amp;t=KhVnzu9r1VwbKPjd-1</t>
+  </si>
+  <si>
+    <t>POC : je lis un epub, ok | Je me déplace d'une page à l'autre et j'apprends à faire du MAUI</t>
   </si>
 </sst>
 </file>
@@ -426,15 +429,15 @@
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1043,10 +1046,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.14583333333333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1974,7 +1977,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2009,11 +2012,11 @@
       <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="C2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
       <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
@@ -2027,7 +2030,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 0 heurs 30 minutes</v>
+        <v>0 jours 7 heurs 0 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2042,24 +2045,24 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>30</v>
+        <v>420</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="55"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" spans="1:15" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21" t="s">
@@ -2112,15 +2115,19 @@
       <c r="B8" s="39">
         <v>45369</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="43"/>
+      <c r="C8" s="35">
+        <v>3</v>
+      </c>
+      <c r="D8" s="43">
+        <v>0</v>
+      </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="54" t="s">
         <v>31</v>
       </c>
       <c r="M8" t="s">
@@ -2134,15 +2141,25 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="str">
+      <c r="A9" s="14">
         <f>IF(ISBLANK(B9),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B9))</f>
-        <v/>
-      </c>
-      <c r="B9" s="40"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="48"/>
+        <v>13</v>
+      </c>
+      <c r="B9" s="40">
+        <v>45376</v>
+      </c>
+      <c r="C9" s="36">
+        <v>3</v>
+      </c>
+      <c r="D9" s="44">
+        <v>30</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="20"/>
       <c r="M9" t="s">
         <v>4</v>
@@ -8267,7 +8284,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
@@ -8279,17 +8296,17 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C6,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C6" s="29" t="str">
         <f>'Journal de travail'!M10</f>
@@ -8297,7 +8314,7 @@
       </c>
       <c r="D6" s="45">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -8388,7 +8405,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>2.0833333333333332E-2</v>
+        <v>0.29166666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8667,6 +8684,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8676,15 +8702,6 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8708,6 +8725,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8719,12 +8744,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add connection page and homeMenu page
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3A9BFF-B0A8-4D16-92C7-E7E20A1E06C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C8047A-9EDF-444D-B816-E30CCB6FE01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -139,6 +139,12 @@
   </si>
   <si>
     <t>POC : je lis un epub, ok | Je me déplace d'une page à l'autre et j'apprends à faire du MAUI</t>
+  </si>
+  <si>
+    <t>Créer un fond d'écran d'une certaine couleur</t>
+  </si>
+  <si>
+    <t>Créer la page de connexion et d'accueil</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.125</c:v>
+                  <c:v>0.1875</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333334</c:v>
@@ -1977,7 +1983,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2030,7 +2036,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 7 heurs 0 minutes</v>
+        <v>0 jours 8 heurs 30 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2049,11 +2055,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>420</v>
+        <v>510</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2172,14 +2178,23 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="str">
+      <c r="A10" s="14">
         <f>IF(ISBLANK(B10),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B10))</f>
-        <v/>
-      </c>
-      <c r="B10" s="39"/>
+        <v>16</v>
+      </c>
+      <c r="B10" s="39">
+        <v>45397</v>
+      </c>
       <c r="C10" s="35"/>
-      <c r="D10" s="43"/>
-      <c r="F10" s="48"/>
+      <c r="D10" s="43">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="48" t="s">
+        <v>33</v>
+      </c>
       <c r="G10" s="17"/>
       <c r="M10" t="s">
         <v>5</v>
@@ -2192,15 +2207,23 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="str">
+      <c r="A11" s="14">
         <f>IF(ISBLANK(B11),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B11))</f>
-        <v/>
-      </c>
-      <c r="B11" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="B11" s="39">
+        <v>45397</v>
+      </c>
       <c r="C11" s="36"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="48"/>
+      <c r="D11" s="44">
+        <v>55</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="48" t="s">
+        <v>34</v>
+      </c>
       <c r="G11" s="20"/>
       <c r="M11" t="s">
         <v>6</v>
@@ -8288,7 +8311,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8296,7 +8319,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.125</v>
+        <v>0.1875</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8405,7 +8428,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.29166666666666669</v>
+        <v>0.35416666666666669</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8684,15 +8707,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8702,6 +8716,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8725,14 +8748,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8744,4 +8759,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Continue creating the home menu
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C8047A-9EDF-444D-B816-E30CCB6FE01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818C6E41-C952-4884-BFC5-DB33273A18BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Créer la page de connexion et d'accueil</t>
+  </si>
+  <si>
+    <t>J'essaie d'afficher le Epub dans MAUI je n'y arrive pas</t>
   </si>
 </sst>
 </file>
@@ -1052,7 +1055,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1875</c:v>
+                  <c:v>0.22569444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333334</c:v>
@@ -1983,7 +1986,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2036,7 +2039,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 8 heurs 30 minutes</v>
+        <v>0 jours 9 heurs 25 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2055,11 +2058,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>150</v>
+        <v>205</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>510</v>
+        <v>565</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2236,14 +2239,23 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="str">
+      <c r="A12" s="14">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="39"/>
+        <v>16</v>
+      </c>
+      <c r="B12" s="39">
+        <v>45397</v>
+      </c>
       <c r="C12" s="35"/>
-      <c r="D12" s="43"/>
-      <c r="F12" s="48"/>
+      <c r="D12" s="43">
+        <v>55</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>35</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8311,7 +8323,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8319,7 +8331,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.1875</v>
+        <v>0.22569444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8428,7 +8440,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.35416666666666669</v>
+        <v>0.3923611111111111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8707,6 +8719,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8716,15 +8737,6 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8748,6 +8760,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8759,12 +8779,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating the diary work
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818C6E41-C952-4884-BFC5-DB33273A18BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682B3D0D-3C5F-4994-895C-94A180E2752F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>J'essaie d'afficher le Epub dans MAUI je n'y arrive pas</t>
+  </si>
+  <si>
+    <t>Je règle une erreur que j'ai eu en essayant de lire un Epub, je n'ai pas compris ce que c'était donc j'ai rechargé une vieille version.</t>
+  </si>
+  <si>
+    <t>J'ai avancé sur ma page d'accueil</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1061,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22569444444444445</c:v>
+                  <c:v>0.25347222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333334</c:v>
@@ -1986,7 +1992,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2045,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 25 minutes</v>
+        <v>0 jours 10 heurs 5 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2058,11 +2064,11 @@
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>565</v>
+        <v>605</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2267,16 +2273,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="str">
+    <row r="13" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="14">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45397</v>
+      </c>
       <c r="C13" s="36"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="48"/>
+      <c r="D13" s="44">
+        <v>30</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="20"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2289,14 +2303,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="14">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="39"/>
+        <v>16</v>
+      </c>
+      <c r="B14" s="39">
+        <v>45397</v>
+      </c>
       <c r="C14" s="35"/>
-      <c r="D14" s="43"/>
-      <c r="F14" s="48"/>
+      <c r="D14" s="43">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="M14" t="s">
         <v>24</v>
@@ -8323,7 +8346,7 @@
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8331,7 +8354,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.22569444444444445</v>
+        <v>0.25347222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8440,7 +8463,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.3923611111111111</v>
+        <v>0.4201388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Continue creating the library menu and parameter menu
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D9288-54B2-4388-AC40-142AB875945A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2870E6-0B4F-4A08-8882-3B1EE74E5676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>Je règle un problème avec GitHub</t>
+  </si>
+  <si>
+    <t>Je crée le menu d'accueil</t>
+  </si>
+  <si>
+    <t>Utiliser Base64 pour convertir/déconvertir en binaire</t>
+  </si>
+  <si>
+    <t>Je crée la structure des livres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser le code ".cs" pour intergair avec le XAML et afficher des images aléatoirement </t>
+  </si>
+  <si>
+    <t>J'avance dans la création des paramètres et de la librairie en même temps</t>
   </si>
 </sst>
 </file>
@@ -343,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -450,6 +465,12 @@
     </xf>
     <xf numFmtId="20" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1058,7 +1079,7 @@
                   <c:v>6.9444444444444441E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22569444444444445</c:v>
+                  <c:v>0.35069444444444442</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333334</c:v>
@@ -1989,7 +2010,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2063,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 35 minutes</v>
+        <v>0 jours 12 heurs 35 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2057,15 +2078,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>215</v>
+        <v>275</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>575</v>
+        <v>755</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2300,15 +2321,26 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="str">
+      <c r="A14" s="14">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="43"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="17"/>
+        <v>17</v>
+      </c>
+      <c r="B14" s="39">
+        <v>45404</v>
+      </c>
+      <c r="C14" s="35">
+        <v>1</v>
+      </c>
+      <c r="D14" s="43">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="57"/>
       <c r="M14" t="s">
         <v>24</v>
       </c>
@@ -2320,16 +2352,24 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="str">
+      <c r="A15" s="14">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="40"/>
+        <v>17</v>
+      </c>
+      <c r="B15" s="40">
+        <v>45404</v>
+      </c>
       <c r="C15" s="36"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="20"/>
+      <c r="D15" s="44">
+        <v>20</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="58"/>
       <c r="M15" t="s">
         <v>25</v>
       </c>
@@ -2341,29 +2381,48 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="str">
+      <c r="A16" s="14">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="39"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="39">
+        <v>45404</v>
+      </c>
       <c r="C16" s="35"/>
-      <c r="D16" s="43"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="17"/>
+      <c r="D16" s="43">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="57"/>
       <c r="O16">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="str">
+      <c r="A17" s="14">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="48"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="40">
+        <v>45404</v>
+      </c>
+      <c r="C17" s="36">
+        <v>1</v>
+      </c>
+      <c r="D17" s="44">
+        <v>10</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="48" t="s">
+        <v>41</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="O17">
         <v>45</v>
@@ -2442,7 +2501,9 @@
       <c r="D23" s="44"/>
       <c r="E23" s="19"/>
       <c r="F23" s="48"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="20" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="str">
@@ -8330,11 +8391,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>180</v>
+        <v>300</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>145</v>
+        <v>205</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8342,7 +8403,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.22569444444444445</v>
+        <v>0.35069444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8451,7 +8512,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.39930555555555552</v>
+        <v>0.52430555555555558</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Connect to the database of the API
</commit_message>
<xml_diff>
--- a/doc/Journal-de-Travail_BerchelJoachim.xlsx
+++ b/doc/Journal-de-Travail_BerchelJoachim.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\px59nyu\Documents\GitHub\readingPassion\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{810A4A96-35AD-4A0E-83A0-90CD3BE86179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2B1904-478C-497B-9A7A-ACD6544EBE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="54">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -191,6 +191,18 @@
   </si>
   <si>
     <t>Mettre en place l'API et un container docker pour la DB</t>
+  </si>
+  <si>
+    <t>J'essaie de récupérer un document txt stocké dans Resources/Raw dans mon application depuis le téléphone. Sans succès</t>
+  </si>
+  <si>
+    <t>J'essaie de faire la connection à la base de donnée. Je n'ai pas réussi. Je vais essayer d'utiliser le "helper" du marketplace</t>
+  </si>
+  <si>
+    <t>J'ai réussi à faire la connexion à la base de donnée grâce au helper</t>
+  </si>
+  <si>
+    <t>J'affiche les données récupérés dans la base de donnée</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1119,7 @@
                   <c:v>1.7361111111111112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47916666666666669</c:v>
+                  <c:v>0.59722222222222221</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.14583333333333334</c:v>
@@ -2037,8 +2049,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <pane ySplit="6" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2103,7 @@
       </c>
       <c r="C3" s="25" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 18 heurs 54 minutes</v>
+        <v>0 jours 21 heurs 45 minutes</v>
       </c>
       <c r="D3" s="25"/>
       <c r="E3" s="3"/>
@@ -2106,15 +2118,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="25">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>600</v>
+        <v>720</v>
       </c>
       <c r="D4" s="25">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>535</v>
+        <v>585</v>
       </c>
       <c r="E4" s="52">
         <f>SUM(C4:D4)</f>
-        <v>1135</v>
+        <v>1305</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2628,55 +2640,88 @@
       </c>
       <c r="G25" s="20"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="str">
+    <row r="26" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="14">
         <f>IF(ISBLANK(B26),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B26))</f>
-        <v/>
-      </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="35"/>
+        <v>22</v>
+      </c>
+      <c r="B26" s="39">
+        <v>45439</v>
+      </c>
+      <c r="C26" s="35">
+        <v>1</v>
+      </c>
       <c r="D26" s="43">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
       </c>
-      <c r="F26" s="48"/>
+      <c r="F26" s="48" t="s">
+        <v>50</v>
+      </c>
       <c r="G26" s="17"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="str">
+    <row r="27" spans="1:15" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14">
         <f>IF(ISBLANK(B27),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B27))</f>
-        <v/>
-      </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="48"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="40">
+        <v>45439</v>
+      </c>
+      <c r="C27" s="36">
+        <v>1</v>
+      </c>
+      <c r="D27" s="44">
+        <v>0</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" s="48" t="s">
+        <v>51</v>
+      </c>
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="str">
+      <c r="A28" s="14">
         <f>IF(ISBLANK(B28),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B28))</f>
-        <v/>
-      </c>
-      <c r="B28" s="39"/>
+        <v>22</v>
+      </c>
+      <c r="B28" s="39">
+        <v>45439</v>
+      </c>
       <c r="C28" s="35"/>
-      <c r="D28" s="43"/>
-      <c r="F28" s="47"/>
+      <c r="D28" s="43">
+        <v>35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="47" t="s">
+        <v>52</v>
+      </c>
       <c r="G28" s="17"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="str">
+      <c r="A29" s="14">
         <f>IF(ISBLANK(B29),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B29))</f>
-        <v/>
-      </c>
-      <c r="B29" s="40"/>
+        <v>22</v>
+      </c>
+      <c r="B29" s="40">
+        <v>45439</v>
+      </c>
       <c r="C29" s="36"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="47"/>
+      <c r="D29" s="44">
+        <v>25</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" s="47" t="s">
+        <v>53</v>
+      </c>
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8496,11 +8541,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>240</v>
+        <v>360</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>450</v>
+        <v>500</v>
       </c>
       <c r="C5" s="53" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8508,7 +8553,7 @@
       </c>
       <c r="D5" s="45">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.47916666666666669</v>
+        <v>0.59722222222222221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8617,7 +8662,7 @@
       </c>
       <c r="D12" s="46">
         <f>SUM(D4:D11)</f>
-        <v>0.66319444444444453</v>
+        <v>0.78125000000000011</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8896,15 +8941,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f7d9f5a6-831d-4621-8c77-cbcaf993e406" xsi:nil="true"/>
@@ -8914,6 +8950,15 @@
     <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8937,14 +8982,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -8956,4 +8993,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>